<commit_message>
working on particle system ompf import export
</commit_message>
<xml_diff>
--- a/doc/OMPF-Format.xlsx
+++ b/doc/OMPF-Format.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="179">
   <si>
     <t>string</t>
   </si>
@@ -570,6 +570,27 @@
   </si>
   <si>
     <t>the emitter type (Mesh is not yet supported)</t>
+  </si>
+  <si>
+    <t>max particle count</t>
+  </si>
+  <si>
+    <t>the maximum of particles that exist in parallel within this particle system</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>loop on/off</t>
+  </si>
+  <si>
+    <t>if true the particle system runs in an endless loop</t>
+  </si>
+  <si>
+    <t>emitterID</t>
+  </si>
+  <si>
+    <t>node id of emitter</t>
   </si>
 </sst>
 </file>
@@ -1061,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G213"/>
+  <dimension ref="A1:G216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2762,35 +2783,73 @@
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C130" s="1"/>
-      <c r="E130" s="1"/>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C131" s="1"/>
-      <c r="E131" s="1"/>
+      <c r="A130" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B130" s="9"/>
+      <c r="C130" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="9"/>
+      <c r="G130" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B131" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E131" s="2">
+        <v>2</v>
+      </c>
+      <c r="F131" s="3">
+        <v>500</v>
+      </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C132" s="1"/>
-      <c r="E132" s="1"/>
+      <c r="B132" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E132" s="2">
+        <v>1</v>
+      </c>
+      <c r="F132" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C133" s="1"/>
-      <c r="E133" s="1"/>
+      <c r="B133" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F133" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A134" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B134" s="9"/>
-      <c r="C134" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D134" s="9"/>
-      <c r="E134" s="9"/>
-      <c r="F134" s="9"/>
-      <c r="G134" s="9" t="s">
-        <v>168</v>
-      </c>
+      <c r="C134" s="1"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C135" s="1"/>
@@ -2807,80 +2866,80 @@
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C139" s="1"/>
     </row>
-    <row r="140" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A140" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D140" s="1"/>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C140" s="1"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C141" s="1"/>
-      <c r="D141" s="1"/>
-    </row>
-    <row r="142" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A142" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D142" s="1"/>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C143" s="1"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C142" s="1"/>
+    </row>
+    <row r="143" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A143" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D143" s="1"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C144" s="1"/>
-    </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C145" s="1"/>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D144" s="1"/>
+    </row>
+    <row r="145" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A145" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D145" s="1"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C146" s="1"/>
     </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C147" s="1"/>
     </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C148" s="1"/>
     </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C150" s="1"/>
     </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C151" s="1"/>
     </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C152" s="1"/>
     </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C153" s="1"/>
     </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C154" s="1"/>
     </row>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C155" s="1"/>
     </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C156" s="1"/>
     </row>
-    <row r="157" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C157" s="1"/>
     </row>
-    <row r="158" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C158" s="1"/>
     </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C159" s="1"/>
     </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C160" s="1"/>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.2">
@@ -3041,6 +3100,15 @@
     </row>
     <row r="213" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C213" s="1"/>
+    </row>
+    <row r="214" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C214" s="1"/>
+    </row>
+    <row r="215" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C215" s="1"/>
+    </row>
+    <row r="216" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C216" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>

</xml_diff>

<commit_message>
importing exporting color gradient in ompf
</commit_message>
<xml_diff>
--- a/doc/OMPF-Format.xlsx
+++ b/doc/OMPF-Format.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="184">
   <si>
     <t>string</t>
   </si>
@@ -591,6 +591,21 @@
   </si>
   <si>
     <t>node id of emitter</t>
+  </si>
+  <si>
+    <t>gradients</t>
+  </si>
+  <si>
+    <t>2 byte lenght + float32 pos value pairs</t>
+  </si>
+  <si>
+    <t>iaGradientColor4f</t>
+  </si>
+  <si>
+    <t>color gradient</t>
+  </si>
+  <si>
+    <t>gradient</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1100,7 @@
   <dimension ref="A1:G216"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="F132" sqref="F132"/>
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1139,6 +1154,14 @@
         <v>67</v>
       </c>
     </row>
+    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="F9" s="2"/>
@@ -2849,7 +2872,21 @@
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C134" s="1"/>
+      <c r="B134" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C135" s="1"/>

</xml_diff>

<commit_message>
added more attributes to particle system import export
</commit_message>
<xml_diff>
--- a/doc/OMPF-Format.xlsx
+++ b/doc/OMPF-Format.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="190">
   <si>
     <t>string</t>
   </si>
@@ -587,12 +587,6 @@
     <t>if true the particle system runs in an endless loop</t>
   </si>
   <si>
-    <t>emitterID</t>
-  </si>
-  <si>
-    <t>node id of emitter</t>
-  </si>
-  <si>
     <t>gradients</t>
   </si>
   <si>
@@ -606,6 +600,30 @@
   </si>
   <si>
     <t>gradient</t>
+  </si>
+  <si>
+    <t>iaGradientf</t>
+  </si>
+  <si>
+    <t>emission gradient</t>
+  </si>
+  <si>
+    <t>min vortex torque</t>
+  </si>
+  <si>
+    <t>max vortex torque</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>min vortex range</t>
+  </si>
+  <si>
+    <t>max vortex range</t>
+  </si>
+  <si>
+    <t>vortex check range</t>
   </si>
 </sst>
 </file>
@@ -1097,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G216"/>
+  <dimension ref="A1:G223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1156,10 +1174,10 @@
     </row>
     <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2856,30 +2874,30 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B133" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F133" s="3">
-        <v>0</v>
+        <v>180</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B134" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="D134" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>44</v>
@@ -2895,44 +2913,82 @@
       <c r="C136" s="1"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B137" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="C137" s="1"/>
+      <c r="D137" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E137" s="2">
+        <v>4</v>
+      </c>
+      <c r="F137" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B138" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="C138" s="1"/>
+      <c r="D138" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E138" s="2">
+        <v>4</v>
+      </c>
+      <c r="F138" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B139" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="C139" s="1"/>
+      <c r="D139" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E139" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B140" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="C140" s="1"/>
+      <c r="D140" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E140" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B141" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="C141" s="1"/>
+      <c r="D141" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E141" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C142" s="1"/>
     </row>
-    <row r="143" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A143" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D143" s="1"/>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C143" s="1"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C144" s="1"/>
-      <c r="D144" s="1"/>
-    </row>
-    <row r="145" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A145" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D145" s="1"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C145" s="1"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C146" s="1"/>
@@ -2946,14 +3002,27 @@
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C150" s="1"/>
+    <row r="150" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D150" s="1"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C151" s="1"/>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C152" s="1"/>
+      <c r="D151" s="1"/>
+    </row>
+    <row r="152" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D152" s="1"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C153" s="1"/>
@@ -3146,6 +3215,27 @@
     </row>
     <row r="216" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C216" s="1"/>
+    </row>
+    <row r="217" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C217" s="1"/>
+    </row>
+    <row r="218" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C218" s="1"/>
+    </row>
+    <row r="219" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C219" s="1"/>
+    </row>
+    <row r="220" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C220" s="1"/>
+    </row>
+    <row r="221" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C221" s="1"/>
+    </row>
+    <row r="222" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C222" s="1"/>
+    </row>
+    <row r="223" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C223" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>

</xml_diff>

<commit_message>
added more paramers to particle system import export
</commit_message>
<xml_diff>
--- a/doc/OMPF-Format.xlsx
+++ b/doc/OMPF-Format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\3rd\Igor\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\Igor\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="192">
   <si>
     <t>string</t>
   </si>
@@ -624,6 +624,12 @@
   </si>
   <si>
     <t>vortex check range</t>
+  </si>
+  <si>
+    <t>first texture tiling columns</t>
+  </si>
+  <si>
+    <t>first texture tiling rows</t>
   </si>
 </sst>
 </file>
@@ -1117,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2953,6 +2959,9 @@
       <c r="E139" s="2">
         <v>4</v>
       </c>
+      <c r="F139" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B140" s="1" t="s">
@@ -2965,6 +2974,9 @@
       <c r="E140" s="2">
         <v>4</v>
       </c>
+      <c r="F140" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B141" s="1" t="s">
@@ -2977,12 +2989,39 @@
       <c r="E141" s="2">
         <v>1</v>
       </c>
+      <c r="F141" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B142" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="C142" s="1"/>
+      <c r="D142" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E142" s="2">
+        <v>1</v>
+      </c>
+      <c r="F142" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B143" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="C143" s="1"/>
+      <c r="D143" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E143" s="2">
+        <v>1</v>
+      </c>
+      <c r="F143" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C144" s="1"/>

</xml_diff>

<commit_message>
#95 adding alpha to mesh chunk in OMPF
</commit_message>
<xml_diff>
--- a/doc/OMPF-Format.xlsx
+++ b/doc/OMPF-Format.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="211">
   <si>
     <t>string</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>byte</t>
-  </si>
-  <si>
-    <t>TODO</t>
   </si>
   <si>
     <t>Group Chunk</t>
@@ -92,9 +89,6 @@
   </si>
   <si>
     <t>similar to switch chunk but the application can decide which LODs to show even in parallel</t>
-  </si>
-  <si>
-    <t>not used just the base type definition. All other chunks derive from this</t>
   </si>
   <si>
     <t>type</t>
@@ -345,19 +339,7 @@
     <t>texture 1 … texture n</t>
   </si>
   <si>
-    <t>bounding sphere position</t>
-  </si>
-  <si>
-    <t>bounding sphere radius</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float32 </t>
-  </si>
-  <si>
     <t>texture count</t>
-  </si>
-  <si>
-    <t>0,0,0</t>
   </si>
   <si>
     <t>deprecated</t>
@@ -535,10 +517,6 @@
   </si>
   <si>
     <t>0.0f</t>
-  </si>
-  <si>
-    <t>TODO would be nice to have texture coord mapped on specific textures and texture units
-TODO split target material from mesh; move everythign that is not mesh in to something like Object or Mesh Node and let it refer to the mesh</t>
   </si>
   <si>
     <t>Emitter-Chunk</t>
@@ -681,6 +659,45 @@
   </si>
   <si>
     <t>Transform Chunk 64 bit</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>alpha value 0.0f-1.0f</t>
+  </si>
+  <si>
+    <t>1.0f</t>
+  </si>
+  <si>
+    <t>vertex data size in vertex count</t>
+  </si>
+  <si>
+    <t>index data size in index count</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TODO would be nice to have texture coord mapped on specific textures and texture units
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>TODO split target material from mesh; move everythign that is not mesh in to something like Object or Mesh Node and let it refer to the mesh</t>
+    </r>
+  </si>
+  <si>
+    <t>Particle System</t>
+  </si>
+  <si>
+    <t>Emitter for particles</t>
+  </si>
+  <si>
+    <t>This Chunk type is not actually used. It's just the base type definition. All other chunks derive from it</t>
   </si>
 </sst>
 </file>
@@ -774,7 +791,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -825,15 +842,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1144,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G229"/>
+  <dimension ref="A1:G228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1165,16 +1173,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -1182,15 +1190,15 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1198,15 +1206,15 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1223,19 +1231,19 @@
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
@@ -1246,7 +1254,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="2">
         <v>4</v>
@@ -1257,7 +1265,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2">
         <v>4</v>
@@ -1268,7 +1276,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
@@ -1277,12 +1285,12 @@
         <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17" s="2">
         <v>2</v>
@@ -1306,16 +1314,16 @@
         <v>3</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>5</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -1324,30 +1332,30 @@
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10" t="s">
-        <v>23</v>
+        <v>210</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="9"/>
       <c r="F20" s="11"/>
       <c r="G20" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1355,13 +1363,13 @@
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>8</v>
@@ -1369,16 +1377,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F23" s="3">
         <v>0</v>
@@ -1386,16 +1394,16 @@
     </row>
     <row r="24" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F24" s="3">
         <v>0</v>
@@ -1403,17 +1411,17 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1426,87 +1434,87 @@
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="9"/>
       <c r="F27" s="11"/>
       <c r="G27" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E28" s="2">
         <v>4</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E29" s="2">
         <v>1</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E30" s="2">
         <v>1</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E31" s="2">
         <v>1</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E32" s="2">
         <v>1</v>
@@ -1518,13 +1526,13 @@
     </row>
     <row r="33" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E33" s="2">
         <v>1</v>
@@ -1536,13 +1544,13 @@
     </row>
     <row r="34" spans="1:7" ht="57" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E34" s="2">
         <v>1</v>
@@ -1554,13 +1562,13 @@
     </row>
     <row r="35" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E35" s="2">
         <v>1</v>
@@ -1572,13 +1580,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E36" s="2">
         <v>1</v>
@@ -1590,19 +1598,19 @@
     </row>
     <row r="37" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E37" s="2">
         <v>6</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1611,7 +1619,7 @@
         <v>Base Chunk</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>8</v>
@@ -1623,7 +1631,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -1631,12 +1639,12 @@
       <c r="E40" s="9"/>
       <c r="F40" s="11"/>
       <c r="G40" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C41" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D41" s="1"/>
     </row>
@@ -1646,17 +1654,17 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="9"/>
       <c r="F43" s="11"/>
       <c r="G43" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1665,7 +1673,7 @@
         <v>Base Chunk</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>8</v>
@@ -1673,74 +1681,74 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E45" s="2">
         <f>4*4</f>
         <v>16</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E46" s="2">
         <f>4*4</f>
         <v>16</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E47" s="2">
         <f>4*4</f>
         <v>16</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E48" s="2">
         <f>4*4</f>
         <v>16</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1749,17 +1757,17 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="9"/>
       <c r="F50" s="11"/>
       <c r="G50" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1768,7 +1776,7 @@
         <v>Base Chunk</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>8</v>
@@ -1776,19 +1784,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1797,17 +1805,17 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="9" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1816,7 +1824,7 @@
         <v>Base Chunk</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>8</v>
@@ -1824,13 +1832,13 @@
     </row>
     <row r="56" spans="1:7" ht="57" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E56" s="2">
         <v>1</v>
@@ -1841,32 +1849,32 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="14" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1875,7 +1883,7 @@
         <v>Base Chunk</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>8</v>
@@ -1883,16 +1891,16 @@
     </row>
     <row r="61" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B61" s="16" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F61" s="17">
         <v>0</v>
@@ -1900,10 +1908,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>10</v>
@@ -1912,15 +1920,15 @@
         <v>3</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>10</v>
@@ -1929,15 +1937,15 @@
         <v>3</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>10</v>
@@ -1946,15 +1954,15 @@
         <v>3</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>10</v>
@@ -1963,52 +1971,52 @@
         <v>3</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E66" s="2">
         <v>4</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>89</v>
+        <v>202</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>115</v>
+        <v>203</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E67" s="2">
-        <v>1</v>
-      </c>
-      <c r="F67" s="3">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E68" s="2">
         <v>1</v>
@@ -2019,13 +2027,13 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E69" s="2">
         <v>1</v>
@@ -2034,15 +2042,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>118</v>
+        <v>89</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E70" s="2">
         <v>1</v>
@@ -2051,310 +2059,312 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B71" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="C71" s="19"/>
-      <c r="D71" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E71" s="18">
-        <v>12</v>
-      </c>
-      <c r="F71" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B72" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="E72" s="18">
-        <v>4</v>
-      </c>
-      <c r="F72" s="20">
+    <row r="71" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B71" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E71" s="2">
+        <v>1</v>
+      </c>
+      <c r="F71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B72" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="2">
+        <v>1</v>
+      </c>
+      <c r="F72" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E73" s="2">
-        <v>1</v>
-      </c>
-      <c r="F73" s="3">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F74" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" s="2">
+        <v>4</v>
+      </c>
+      <c r="F74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="B75" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B75" s="1" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B76" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E76" s="2">
+        <v>4</v>
+      </c>
+      <c r="F76" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="B77" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E75" s="2">
-        <v>4</v>
-      </c>
-      <c r="F75" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="B76" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F76" s="3" t="s">
+      <c r="C77" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F77" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B77" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E77" s="2">
-        <v>4</v>
-      </c>
-      <c r="F77" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="B78" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-    </row>
-    <row r="80" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A80" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B80" s="9"/>
-      <c r="C80" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B81" s="1" t="str">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+    </row>
+    <row r="79" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" s="9"/>
+      <c r="C79" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B80" s="1" t="str">
         <f>$A$20</f>
         <v>Base Chunk</v>
       </c>
-      <c r="E81" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B82" s="1" t="s">
+      <c r="E80" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B81" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E82" s="15">
+        <v>1</v>
+      </c>
+      <c r="F82" s="17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B83" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E83" s="2">
+        <v>1</v>
+      </c>
+      <c r="F83" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B84" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="D84" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E84" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B85" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="D83" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E83" s="15">
-        <v>1</v>
-      </c>
-      <c r="F83" s="17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B84" s="1" t="s">
+      <c r="C85" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B86" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E84" s="2">
-        <v>1</v>
-      </c>
-      <c r="F84" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B85" s="1" t="s">
+      <c r="C86" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E86" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B87" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E85" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B86" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B87" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C87" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E87" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B88" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B89" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E89" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B90" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E90" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B91" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>71</v>
+        <v>23</v>
+      </c>
+      <c r="E91" s="2">
+        <v>1</v>
+      </c>
+      <c r="F91" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B92" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E92" s="2">
         <v>1</v>
@@ -2365,11 +2375,11 @@
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B93" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E93" s="2">
         <v>1</v>
@@ -2380,11 +2390,11 @@
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B94" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E94" s="2">
         <v>1</v>
@@ -2395,11 +2405,11 @@
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B95" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E95" s="2">
         <v>1</v>
@@ -2410,11 +2420,11 @@
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B96" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E96" s="2">
         <v>1</v>
@@ -2425,11 +2435,11 @@
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B97" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E97" s="2">
         <v>1</v>
@@ -2440,11 +2450,11 @@
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B98" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E98" s="2">
         <v>1</v>
@@ -2455,11 +2465,11 @@
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B99" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E99" s="2">
         <v>1</v>
@@ -2470,11 +2480,11 @@
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B100" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E100" s="2">
         <v>1</v>
@@ -2485,11 +2495,11 @@
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B101" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E101" s="2">
         <v>1</v>
@@ -2500,11 +2510,11 @@
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B102" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E102" s="2">
         <v>1</v>
@@ -2515,11 +2525,11 @@
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B103" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E103" s="2">
         <v>1</v>
@@ -2530,11 +2540,11 @@
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B104" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E104" s="2">
         <v>1</v>
@@ -2545,11 +2555,11 @@
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B105" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E105" s="2">
         <v>1</v>
@@ -2560,11 +2570,11 @@
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B106" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E106" s="2">
         <v>1</v>
@@ -2575,11 +2585,11 @@
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B107" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E107" s="2">
         <v>1</v>
@@ -2590,11 +2600,11 @@
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B108" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E108" s="2">
         <v>1</v>
@@ -2605,11 +2615,11 @@
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B109" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E109" s="2">
         <v>1</v>
@@ -2620,11 +2630,10 @@
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B110" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E110" s="2">
         <v>1</v>
@@ -2635,10 +2644,10 @@
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B111" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E111" s="2">
         <v>1</v>
@@ -2649,10 +2658,10 @@
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B112" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E112" s="2">
         <v>1</v>
@@ -2663,10 +2672,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B113" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E113" s="2">
         <v>1</v>
@@ -2677,10 +2686,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B114" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E114" s="2">
         <v>1</v>
@@ -2691,10 +2700,10 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B115" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E115" s="2">
         <v>1</v>
@@ -2705,10 +2714,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B116" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E116" s="2">
         <v>1</v>
@@ -2719,10 +2728,10 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B117" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E117" s="2">
         <v>1</v>
@@ -2733,10 +2742,10 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B118" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E118" s="2">
         <v>1</v>
@@ -2747,10 +2756,10 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B119" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E119" s="2">
         <v>1</v>
@@ -2761,10 +2770,10 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B120" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E120" s="2">
         <v>1</v>
@@ -2774,151 +2783,154 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B121" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E121" s="2">
-        <v>1</v>
-      </c>
-      <c r="F121" s="3">
-        <v>0</v>
-      </c>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
+      <c r="A123" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B123" s="9"/>
+      <c r="C123" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D123" s="9"/>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="9" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A124" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B124" s="9"/>
-      <c r="C124" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D124" s="9"/>
-      <c r="E124" s="9"/>
-      <c r="F124" s="9"/>
-      <c r="G124" s="9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B125" s="1" t="str">
+      <c r="B124" s="1" t="str">
         <f>$A$20</f>
         <v>Base Chunk</v>
       </c>
-      <c r="E125" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F125" s="3" t="s">
+      <c r="E124" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F124" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="B125" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E125" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B126" s="1" t="s">
-        <v>4</v>
+        <v>161</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>56</v>
+        <v>163</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E126" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B127" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E127" s="1">
-        <v>1</v>
-      </c>
+      <c r="C127" s="1"/>
+      <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C128" s="1"/>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C129" s="1"/>
-      <c r="E129" s="1"/>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" s="9" t="s">
+      <c r="A129" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B129" s="9"/>
+      <c r="C129" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="9"/>
+      <c r="G129" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B130" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B130" s="9"/>
-      <c r="C130" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D130" s="9"/>
-      <c r="E130" s="9"/>
-      <c r="F130" s="9"/>
-      <c r="G130" s="9" t="s">
+      <c r="D130" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E130" s="2">
+        <v>2</v>
+      </c>
+      <c r="F130" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B131" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B131" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="C131" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>25</v>
+        <v>166</v>
       </c>
       <c r="E131" s="2">
-        <v>2</v>
-      </c>
-      <c r="F131" s="3">
-        <v>500</v>
+        <v>1</v>
+      </c>
+      <c r="F131" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B132" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E132" s="2">
-        <v>1</v>
-      </c>
-      <c r="F132" s="3" t="b">
-        <v>1</v>
+      <c r="E132" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B133" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F133" s="3" t="s">
         <v>8</v>
@@ -2926,16 +2938,16 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B134" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F134" s="3" t="s">
         <v>8</v>
@@ -2943,16 +2955,16 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B135" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F135" s="3" t="s">
         <v>8</v>
@@ -2960,16 +2972,16 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B136" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F136" s="3" t="s">
         <v>8</v>
@@ -2977,16 +2989,16 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B137" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F137" s="3" t="s">
         <v>8</v>
@@ -2994,16 +3006,16 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B138" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F138" s="3" t="s">
         <v>8</v>
@@ -3011,16 +3023,16 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B139" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F139" s="3" t="s">
         <v>8</v>
@@ -3028,28 +3040,26 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B140" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>192</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="C140" s="1"/>
       <c r="D140" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E140" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F140" s="3" t="s">
-        <v>8</v>
+        <v>178</v>
+      </c>
+      <c r="E140" s="2">
+        <v>4</v>
+      </c>
+      <c r="F140" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B141" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E141" s="2">
         <v>4</v>
@@ -3060,11 +3070,11 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B142" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E142" s="2">
         <v>4</v>
@@ -3075,11 +3085,11 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B143" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E143" s="2">
         <v>4</v>
@@ -3090,14 +3100,14 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B144" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="2" t="s">
-        <v>185</v>
+        <v>23</v>
       </c>
       <c r="E144" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F144" s="3">
         <v>0</v>
@@ -3105,14 +3115,14 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B145" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="2" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="E145" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F145" s="3">
         <v>0</v>
@@ -3120,11 +3130,11 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B146" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E146" s="2">
         <v>4</v>
@@ -3135,26 +3145,26 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B147" s="1" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="2" t="s">
-        <v>185</v>
+        <v>23</v>
       </c>
       <c r="E147" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F147" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B148" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C148" s="1"/>
       <c r="D148" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E148" s="2">
         <v>1</v>
@@ -3165,26 +3175,26 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B149" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="2" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="E149" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F149" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B150" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C150" s="1"/>
       <c r="D150" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E150" s="2">
         <v>4</v>
@@ -3195,120 +3205,108 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B151" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C151" s="1"/>
       <c r="D151" s="2" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="E151" s="2">
-        <v>4</v>
-      </c>
-      <c r="F151" s="3">
+        <v>1</v>
+      </c>
+      <c r="F151" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B152" s="1" t="s">
-        <v>202</v>
+        <v>101</v>
       </c>
       <c r="C152" s="1"/>
-      <c r="D152" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E152" s="2">
-        <v>1</v>
-      </c>
-      <c r="F152" s="3" t="b">
-        <v>0</v>
+      <c r="D152" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B153" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="C153" s="1"/>
-      <c r="D153" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F153" s="3" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C154" s="1"/>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C155" s="1"/>
-    </row>
-    <row r="156" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A156" s="2" t="s">
+    <row r="155" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D155" s="1"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C156" s="1"/>
+      <c r="D156" s="1"/>
+    </row>
+    <row r="157" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A157" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C157" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D156" s="1"/>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C157" s="1"/>
       <c r="D157" s="1"/>
     </row>
-    <row r="158" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A158" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D158" s="1"/>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C158" s="1"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
+        <v>197</v>
+      </c>
       <c r="C159" s="1"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A160" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="C160" s="1"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="C161" s="1"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A162" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="C162" s="1"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="C163" s="1"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A164" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="C164" s="1"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
+        <v>200</v>
+      </c>
       <c r="C165" s="1"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A166" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="C166" s="1"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" s="2" t="s">
+        <v>201</v>
+      </c>
       <c r="C167" s="1"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A168" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="C168" s="1"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
@@ -3490,9 +3488,6 @@
     </row>
     <row r="228" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C228" s="1"/>
-    </row>
-    <row r="229" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C229" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>

</xml_diff>